<commit_message>
Updated Alf_Messages (changed datatype of angle and use same names as in implementation)
</commit_message>
<xml_diff>
--- a/Documentation/Alf_Messages.xlsx
+++ b/Documentation/Alf_Messages.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Nachrichtendefinitionen Alf'!$A:$H</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Nachrichtendefinitionen Alf'!$A:$H</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Nachrichtendefinitionen Alf'!$A:$H</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t xml:space="preserve">Nachrichtendefinitionen für ALF</t>
   </si>
@@ -181,13 +182,13 @@
     <t xml:space="preserve">uint8_t</t>
   </si>
   <si>
-    <t xml:space="preserve">Sollgeschwindigkeit</t>
+    <t xml:space="preserve">speed</t>
   </si>
   <si>
     <t xml:space="preserve">Geschwindigkeit zwischen 0 und 100, Werte darüber werden als 100% interpretiert</t>
   </si>
   <si>
-    <t xml:space="preserve">Sollrichtung</t>
+    <t xml:space="preserve">direction</t>
   </si>
   <si>
     <t xml:space="preserve">Sollrichtung
@@ -195,16 +196,19 @@
 1 := Rückwärts</t>
   </si>
   <si>
-    <t xml:space="preserve">Lenkwinkel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 – 180°</t>
+    <t xml:space="preserve">int8_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-90 – 90°</t>
   </si>
   <si>
     <t xml:space="preserve">bool</t>
   </si>
   <si>
-    <t xml:space="preserve">Licht</t>
+    <t xml:space="preserve">light</t>
   </si>
   <si>
     <t xml:space="preserve">true: an, false: aus</t>
@@ -213,49 +217,49 @@
     <t xml:space="preserve">Daten vom Fahrzeug zum HQ (alf_drive_info)</t>
   </si>
   <si>
-    <t xml:space="preserve">Geschwindigkeit</t>
-  </si>
-  <si>
     <t xml:space="preserve">0 – Vollgas</t>
   </si>
   <si>
     <t xml:space="preserve">int16_t</t>
   </si>
   <si>
-    <t xml:space="preserve">Beschleunigung</t>
+    <t xml:space="preserve">acceleration</t>
   </si>
   <si>
     <t xml:space="preserve">Beschleunigung in Längsrichtung</t>
   </si>
   <si>
-    <t xml:space="preserve">Querbeschleunigung</t>
+    <t xml:space="preserve">lateral_acceleration</t>
   </si>
   <si>
     <t xml:space="preserve">Beschleunigung in Querrichtung</t>
   </si>
   <si>
-    <t xml:space="preserve">Hochbeschleunigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschleunigung zum Erdinneren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gyroskop X</t>
+    <t xml:space="preserve">z_acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschleunigung in Z-Richtung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gyroscope_X</t>
   </si>
   <si>
     <t xml:space="preserve">Gyroskop in X Richtung</t>
   </si>
   <si>
-    <t xml:space="preserve">Gyroskop Y</t>
+    <t xml:space="preserve">Gyroscope_Y</t>
   </si>
   <si>
     <t xml:space="preserve">Gyroskop in Y Richtung</t>
   </si>
   <si>
-    <t xml:space="preserve">Gyroskop Z</t>
+    <t xml:space="preserve">Gyroscope_Z</t>
   </si>
   <si>
     <t xml:space="preserve">Gyroskop in Z Richtung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature</t>
   </si>
   <si>
     <t xml:space="preserve">Temperatur</t>
@@ -274,11 +278,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -300,25 +303,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -360,24 +344,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -389,6 +361,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66FF00"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -415,7 +393,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -439,32 +417,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,63 +443,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,19 +504,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="hintergrund2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 3" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 4" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Unbenannt1" xfId="25" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -601,7 +537,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -644,24 +580,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="9.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="5.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="69.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="5" width="10.62"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.9023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="17.4279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="39.5348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="10.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="6.2046511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.6837209302326"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="76.2651162790698"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="16.3767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="11.6976744186047"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +611,6 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
       <c r="J1" s="6" t="s">
         <v>1</v>
       </c>
@@ -683,8 +618,6 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -695,14 +628,11 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
@@ -713,14 +643,11 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -731,383 +658,295 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="10" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="H6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="n">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="16" t="n">
+      <c r="D7" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" s="16" t="s">
+      <c r="F7" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="n">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="F8" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="16" t="n">
+      <c r="F9" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="F11" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="17" t="n">
+    </row>
+    <row r="12" s="5" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="16" t="n">
+      <c r="A13" s="5"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="16" t="n">
+      <c r="A14" s="5"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="E15" s="16" t="s">
+      <c r="A15" s="5"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" s="16" t="s">
+      <c r="F15" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="16" t="n">
+      <c r="A16" s="5"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" s="16" t="s">
+      <c r="F16" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="16" t="n">
+      <c r="A17" s="5"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="G17" s="16" t="s">
+      <c r="F17" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="4" t="n">
@@ -1125,17 +964,9 @@
       <c r="H18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="20"/>
+    </row>
+    <row r="19" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="16"/>
       <c r="D19" s="4" t="n">
         <v>2</v>
       </c>
@@ -1151,73 +982,49 @@
       <c r="H19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="20"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="16"/>
       <c r="D20" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="20"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="16"/>
       <c r="D21" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F21" s="4" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>53</v>
+      <c r="C22" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>1</v>
@@ -1229,22 +1036,14 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="20"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="16"/>
       <c r="D23" s="4" t="n">
         <v>2</v>
       </c>
@@ -1260,17 +1059,9 @@
       <c r="H23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="20"/>
+    </row>
+    <row r="24" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="16"/>
       <c r="D24" s="4" t="n">
         <v>3</v>
       </c>
@@ -1286,17 +1077,9 @@
       <c r="H24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="20"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="16"/>
       <c r="D25" s="4" t="n">
         <v>4</v>
       </c>
@@ -1312,17 +1095,9 @@
       <c r="H25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="20"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="n">
         <v>5</v>
       </c>
@@ -1338,17 +1113,9 @@
       <c r="H26" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="20"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="n">
         <v>6</v>
       </c>
@@ -1364,17 +1131,9 @@
       <c r="H27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="20"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="16"/>
       <c r="D28" s="4" t="n">
         <v>7</v>
       </c>
@@ -1390,17 +1149,9 @@
       <c r="H28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="16"/>
       <c r="D29" s="4" t="n">
         <v>8</v>
       </c>
@@ -1414,46 +1165,21 @@
         <v>69</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-    </row>
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="n">
         <v>255</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>1</v>
@@ -1465,19 +1191,11 @@
         <v>1</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>